<commit_message>
feature: add first innovation mgt topic
</commit_message>
<xml_diff>
--- a/public/marketing_innovation_questions.xlsx
+++ b/public/marketing_innovation_questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/innovation-mgt/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrykostern/Documents/code/marketing-and-innovation-mgt/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F0D896-1EE7-A342-9636-911BFC213E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02507D8D-A57C-2048-A81B-8AF1CB211FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principles of Marketing &amp; Ethic" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Marketing Communications" sheetId="10" r:id="rId10"/>
     <sheet name="Marketing Channels" sheetId="11" r:id="rId11"/>
     <sheet name="People, Process, and Physical E" sheetId="12" r:id="rId12"/>
+    <sheet name="Introduction" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3149" uniqueCount="2539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="2723">
   <si>
     <t>Question</t>
   </si>
@@ -7661,6 +7662,558 @@
   </si>
   <si>
     <t>Customer-oriented employees tailor actions to customer requirements.</t>
+  </si>
+  <si>
+    <t>Which definition captures the dual nature of innovation as both process and outcome?</t>
+  </si>
+  <si>
+    <t>A new way of doing things that is commercialized.</t>
+  </si>
+  <si>
+    <t>Innovations are qualitatively new products or processes that differ significantly from what existed before.</t>
+  </si>
+  <si>
+    <t>The adoption of ideas that are new to the adopting organization.</t>
+  </si>
+  <si>
+    <t>Innovation management is the creation of processes that aim at creating and exploiting new things.</t>
+  </si>
+  <si>
+    <t>This definition explicitly refers to innovation as new products/processes (outcome) and implies an underlying process.</t>
+  </si>
+  <si>
+    <t>Porter’s definition of innovation emphasizes:</t>
+  </si>
+  <si>
+    <t>Process-innovation only</t>
+  </si>
+  <si>
+    <t>Commercialization of new methods</t>
+  </si>
+  <si>
+    <t>R&amp;D spending levels</t>
+  </si>
+  <si>
+    <t>Co-creation by multiple actors</t>
+  </si>
+  <si>
+    <t>Porter defines innovation as a new way of doing things that is commercialized.</t>
+  </si>
+  <si>
+    <t>Schumpeter’s concept of “creative destruction” refers to:</t>
+  </si>
+  <si>
+    <t>Continuous improvement of existing products</t>
+  </si>
+  <si>
+    <t>Innovation that undermines established firms by offering decisive cost or quality advantages</t>
+  </si>
+  <si>
+    <t>Government-driven economic growth</t>
+  </si>
+  <si>
+    <t>Incremental process enhancements only</t>
+  </si>
+  <si>
+    <t>Schumpeter argued that new commodities attack existing firms’ foundations.</t>
+  </si>
+  <si>
+    <t>Baumol’s view on innovation under capitalism states that:</t>
+  </si>
+  <si>
+    <t>Innovation is optional for firm survival</t>
+  </si>
+  <si>
+    <t>Price-setting remains the primary competitive tool</t>
+  </si>
+  <si>
+    <t>Innovative activity becomes mandatory for firm success</t>
+  </si>
+  <si>
+    <t>Capital markets hinder innovation efforts</t>
+  </si>
+  <si>
+    <t>Under capitalism, firms must innovate or risk failure.</t>
+  </si>
+  <si>
+    <t>Which statistic reflects the OECD’s view on innovation’s role in productivity?</t>
+  </si>
+  <si>
+    <t>Innovation accounts for 10–20% of labor productivity growth</t>
+  </si>
+  <si>
+    <t>Innovation investments explain 60–70% of labor productivity growth in high-income countries</t>
+  </si>
+  <si>
+    <t>Public R&amp;D funds exceed private R&amp;D</t>
+  </si>
+  <si>
+    <t>Innovation has little impact on employment rates</t>
+  </si>
+  <si>
+    <t>OECD estimates intangible investments drive 60–70% of productivity growth.</t>
+  </si>
+  <si>
+    <t>Dissecting Edison’s “99% perspiration” story shows that:</t>
+  </si>
+  <si>
+    <t>Radical ideas succeed with little effort</t>
+  </si>
+  <si>
+    <t>Systematic experimentation of hundreds of materials is crucial for innovation</t>
+  </si>
+  <si>
+    <t>Innovation depends solely on serendipity</t>
+  </si>
+  <si>
+    <t>Lab workers’ habits are unimportant</t>
+  </si>
+  <si>
+    <t>Edison tested dozens of filaments, illustrating persistence and experimentation.</t>
+  </si>
+  <si>
+    <t>Which type of innovation reshuffles the firm’s value proposition, processes, and revenue logic?</t>
+  </si>
+  <si>
+    <t>Process innovation</t>
+  </si>
+  <si>
+    <t>Business model innovation</t>
+  </si>
+  <si>
+    <t>Incremental innovation</t>
+  </si>
+  <si>
+    <t>Business model innovation reconfigures value creation and capture.</t>
+  </si>
+  <si>
+    <t>Product and process innovations often co-occur because:</t>
+  </si>
+  <si>
+    <t>They are legally required to be linked</t>
+  </si>
+  <si>
+    <t>New products frequently demand new manufacturing processes</t>
+  </si>
+  <si>
+    <t>Customers cannot distinguish them</t>
+  </si>
+  <si>
+    <t>They share identical risk profiles</t>
+  </si>
+  <si>
+    <t>Novel products often require novel production methods.</t>
+  </si>
+  <si>
+    <t>Which phase of R&amp;D receives the largest share of total spending?</t>
+  </si>
+  <si>
+    <t>Market commercialization</t>
+  </si>
+  <si>
+    <t>Experimental development is the bulk of R&amp;D expenditures.</t>
+  </si>
+  <si>
+    <t>Principal-agent problems in innovation projects arise when:</t>
+  </si>
+  <si>
+    <t>Agents and principals share identical incentives</t>
+  </si>
+  <si>
+    <t>Information asymmetry leads agents to pursue their own goals</t>
+  </si>
+  <si>
+    <t>All stakeholders have perfect visibility</t>
+  </si>
+  <si>
+    <t>Innovation always yields certain profits</t>
+  </si>
+  <si>
+    <t>Agents may hide risks or overstate progress when not monitored.</t>
+  </si>
+  <si>
+    <t>Interface problems in innovation teams often stem from:</t>
+  </si>
+  <si>
+    <t>Excessive open communication</t>
+  </si>
+  <si>
+    <t>Team members being punished for voicing concerns</t>
+  </si>
+  <si>
+    <t>Too much top-down oversight</t>
+  </si>
+  <si>
+    <t>Over-funding the project</t>
+  </si>
+  <si>
+    <t>Fear of reprisal stifles dissent, so early warnings go unheard.</t>
+  </si>
+  <si>
+    <t>Which example shows that not every invention becomes an innovation?</t>
+  </si>
+  <si>
+    <t>The mousetrap’s snap-trap design</t>
+  </si>
+  <si>
+    <t>Penicillin production</t>
+  </si>
+  <si>
+    <t>Gas-filled umbrella sketches</t>
+  </si>
+  <si>
+    <t>3D-printed turbine blades</t>
+  </si>
+  <si>
+    <t>Novel ideas failed to find market acceptance.</t>
+  </si>
+  <si>
+    <t>The mousetrap story demonstrates that:</t>
+  </si>
+  <si>
+    <t>First patent always wins the market</t>
+  </si>
+  <si>
+    <t>Simplicity and practicality trump complexity and novelty</t>
+  </si>
+  <si>
+    <t>Thousands of patents guarantee success</t>
+  </si>
+  <si>
+    <t>High-tech solutions outperform low-tech</t>
+  </si>
+  <si>
+    <t>Only simple snap-trap endured among 4,400+ patents.</t>
+  </si>
+  <si>
+    <t>Innovation risk factors include all except:</t>
+  </si>
+  <si>
+    <t>Technological uncertainty</t>
+  </si>
+  <si>
+    <t>Demand uncertainty</t>
+  </si>
+  <si>
+    <t>Competitive uncertainty</t>
+  </si>
+  <si>
+    <t>Guaranteed patent protection</t>
+  </si>
+  <si>
+    <t>Patents help protect but do not remove risks.</t>
+  </si>
+  <si>
+    <t>Why must innovation be managed differently than routine operations?</t>
+  </si>
+  <si>
+    <t>It always follows predictable processes</t>
+  </si>
+  <si>
+    <t>It involves novel, uncertain, and cross-functional activities</t>
+  </si>
+  <si>
+    <t>It never requires cross-departmental cooperation</t>
+  </si>
+  <si>
+    <t>It is immune to market forces</t>
+  </si>
+  <si>
+    <t>Innovation’s uncertainty demands special approaches.</t>
+  </si>
+  <si>
+    <t>Which is a key enabler for firms to secure profits from innovation?</t>
+  </si>
+  <si>
+    <t>Immediate full disclosure</t>
+  </si>
+  <si>
+    <t>Protection mechanisms (patents)</t>
+  </si>
+  <si>
+    <t>No marketing investment</t>
+  </si>
+  <si>
+    <t>Ignoring competition</t>
+  </si>
+  <si>
+    <t>Legal protections help appropriate returns.</t>
+  </si>
+  <si>
+    <t>“Innovation as part of firm strategy” implies:</t>
+  </si>
+  <si>
+    <t>R&amp;D separate from planning</t>
+  </si>
+  <si>
+    <t>Integrating innovation goals into strategy</t>
+  </si>
+  <si>
+    <t>Excluding commercialization</t>
+  </si>
+  <si>
+    <t>Only large firms innovate</t>
+  </si>
+  <si>
+    <t>Leading firms embed innovation in planning.</t>
+  </si>
+  <si>
+    <t>In simplified innovation models, feedback loops are excluded but reality:</t>
+  </si>
+  <si>
+    <t>Phases are sequential</t>
+  </si>
+  <si>
+    <t>Phases overlap and iterate</t>
+  </si>
+  <si>
+    <t>Only invention matters</t>
+  </si>
+  <si>
+    <t>Funding is linear</t>
+  </si>
+  <si>
+    <t>Real projects cycle back between phases.</t>
+  </si>
+  <si>
+    <t>Macro importance of R&amp;D is shown by:</t>
+  </si>
+  <si>
+    <t>Declining global R&amp;D</t>
+  </si>
+  <si>
+    <t>R&amp;D concentration in large firms and economies</t>
+  </si>
+  <si>
+    <t>Equal small-firm R&amp;D</t>
+  </si>
+  <si>
+    <t>R&amp;D’s small productivity role</t>
+  </si>
+  <si>
+    <t>Large firms/OECD dominate global R&amp;D.</t>
+  </si>
+  <si>
+    <t>Which ratio shows basic/applied/development split in R&amp;D budgets?</t>
+  </si>
+  <si>
+    <t>90/10/0</t>
+  </si>
+  <si>
+    <t>5–20/15–25/65–85</t>
+  </si>
+  <si>
+    <t>50/50/0</t>
+  </si>
+  <si>
+    <t>0/0/100</t>
+  </si>
+  <si>
+    <t>Most budgets allocate majority to development.</t>
+  </si>
+  <si>
+    <t>Innovation spillovers refer to:</t>
+  </si>
+  <si>
+    <t>Complete knowledge retention</t>
+  </si>
+  <si>
+    <t>Idea leakage benefiting competitors</t>
+  </si>
+  <si>
+    <t>Licensing revenue</t>
+  </si>
+  <si>
+    <t>Compliance costs</t>
+  </si>
+  <si>
+    <t>Spillovers occur when others build on your innovation.</t>
+  </si>
+  <si>
+    <t>Informal R&amp;D in small firms:</t>
+  </si>
+  <si>
+    <t>Is always captured</t>
+  </si>
+  <si>
+    <t>Often goes unmeasured</t>
+  </si>
+  <si>
+    <t>Exceeds large-firm R&amp;D</t>
+  </si>
+  <si>
+    <t>Never contributes to innovation</t>
+  </si>
+  <si>
+    <t>Small-firm experimentation escapes reporting.</t>
+  </si>
+  <si>
+    <t>The Iridium failure shows technical success can:</t>
+  </si>
+  <si>
+    <t>Ensure acceptance</t>
+  </si>
+  <si>
+    <t>Still fail financially due to pricing misjudgment</t>
+  </si>
+  <si>
+    <t>Require no marketing</t>
+  </si>
+  <si>
+    <t>Succeed on novelty alone</t>
+  </si>
+  <si>
+    <t>High costs and rates deterred users.</t>
+  </si>
+  <si>
+    <t>Which captures modern creative destruction?</t>
+  </si>
+  <si>
+    <t>Protecting legacy products</t>
+  </si>
+  <si>
+    <t>Startups disrupting incumbents</t>
+  </si>
+  <si>
+    <t>Subsidies preventing change</t>
+  </si>
+  <si>
+    <t>Abandoning innovation</t>
+  </si>
+  <si>
+    <t>New entrants disrupt established players.</t>
+  </si>
+  <si>
+    <t>Low-tech can outperform high-tech because:</t>
+  </si>
+  <si>
+    <t>No market fit needed</t>
+  </si>
+  <si>
+    <t>Simpler solutions meet needs reliably</t>
+  </si>
+  <si>
+    <t>No competition</t>
+  </si>
+  <si>
+    <t>No protection needed</t>
+  </si>
+  <si>
+    <t>Simple inventions address core needs effectively.</t>
+  </si>
+  <si>
+    <t>Which is NOT a characteristic of innovation risk?</t>
+  </si>
+  <si>
+    <t>High cost</t>
+  </si>
+  <si>
+    <t>Certainty of success</t>
+  </si>
+  <si>
+    <t>Potential spillovers</t>
+  </si>
+  <si>
+    <t>Need for cooperation</t>
+  </si>
+  <si>
+    <t>Innovation is uncertain by nature.</t>
+  </si>
+  <si>
+    <t>Innovation resistance arises because:</t>
+  </si>
+  <si>
+    <t>Everyone welcomes change</t>
+  </si>
+  <si>
+    <t>Creative destruction threatens routines</t>
+  </si>
+  <si>
+    <t>Innovation requires no change</t>
+  </si>
+  <si>
+    <t>Low costs make adoption easy</t>
+  </si>
+  <si>
+    <t>Destruction unsettles stakeholders.</t>
+  </si>
+  <si>
+    <t>Managing principal-agent in R&amp;D:</t>
+  </si>
+  <si>
+    <t>Reduce transparency</t>
+  </si>
+  <si>
+    <t>Tie incentives to outcomes</t>
+  </si>
+  <si>
+    <t>Prohibit feedback</t>
+  </si>
+  <si>
+    <t>Centralize decisions</t>
+  </si>
+  <si>
+    <t>Metrics and incentives align goals.</t>
+  </si>
+  <si>
+    <t>Why firms innovate beyond profit?</t>
+  </si>
+  <si>
+    <t>Regulation compliance only</t>
+  </si>
+  <si>
+    <t>Competitiveness, growth, societal progress</t>
+  </si>
+  <si>
+    <t>Avoid risk</t>
+  </si>
+  <si>
+    <t>Innovation drives growth and strategic positioning.</t>
+  </si>
+  <si>
+    <t>Value co-creation actors:</t>
+  </si>
+  <si>
+    <t>Firm only</t>
+  </si>
+  <si>
+    <t>Firm and government</t>
+  </si>
+  <si>
+    <t>Firm, customers, suppliers, stakeholders</t>
+  </si>
+  <si>
+    <t>Competitors only</t>
+  </si>
+  <si>
+    <t>Multiple actors collaborate to co-create value.</t>
+  </si>
+  <si>
+    <t>Successful innovation management requires:</t>
+  </si>
+  <si>
+    <t>Routine operations</t>
+  </si>
+  <si>
+    <t>Specialized skills, tools, incentives, structures</t>
+  </si>
+  <si>
+    <t>Perfect forecasting</t>
+  </si>
+  <si>
+    <t>Basic research only</t>
+  </si>
+  <si>
+    <t>Innovation’s unique challenges call for dedicated approaches.</t>
+  </si>
+  <si>
+    <t>Basic research</t>
+  </si>
+  <si>
+    <t>Applied research</t>
+  </si>
+  <si>
+    <t>Experimental development</t>
   </si>
 </sst>
 </file>
@@ -10715,7 +11268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD67C55-784B-6242-B94D-DEA457E2D53E}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -11340,6 +11893,760 @@
       </c>
       <c r="G27" t="s">
         <v>2538</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93EC078-6820-EF43-85BD-74EE81F99F4B}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="63.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2541</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2542</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2543</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2547</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2548</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2549</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2551</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2554</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2555</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2559</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2560</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2561</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2563</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2564</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2565</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2566</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2567</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2571</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2573</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2575</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2409</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2577</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2578</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2580</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2582</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2583</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2584</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2586</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2720</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2721</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2722</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2587</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2589</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2591</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2592</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2593</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2596</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2599</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2601</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2602</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2603</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2604</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2605</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2607</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2608</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2609</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2610</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2611</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2613</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2614</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2615</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2616</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2617</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2618</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2619</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2620</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2622</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2623</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2625</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2628</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2629</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2631</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2632</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2634</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2635</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>2636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2639</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2640</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2644</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2645</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2646</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2647</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2650</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2651</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2652</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2653</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2657</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2658</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2659</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2660</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2662</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2663</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2664</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2665</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2669</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2670</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2671</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>2673</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2674</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2675</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2676</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2677</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>2679</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2680</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2682</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2683</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2686</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2687</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2688</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2689</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2690</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2692</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2695</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2698</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2699</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2700</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2701</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2703</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2704</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2705</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2706</v>
+      </c>
+      <c r="E30" t="s">
+        <v>284</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2709</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2710</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2711</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2712</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2713</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2715</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2716</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2717</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2718</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>